<commit_message>
Update with review process.
</commit_message>
<xml_diff>
--- a/Supplemental Table 1. Average pH of wetland regions.xlsx
+++ b/Supplemental Table 1. Average pH of wetland regions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horto\Documents\Grad School\Central Michigan\Dissertation\Great Lakes Coastal Wetlands\Stats\Final figs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horto\Dropbox\Great Lakes\Manuscript\Submission\Figures and Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,54 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$3:$A$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$H$4:$P$4</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$H$5:$P$5</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$H$6:$P$6</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$F$12:$F$20</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$G$11</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$G$12:$G$20</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$H$11</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$H$12:$H$20</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$I$11</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$I$12:$I$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$3:$B$7</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$J$11</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$J$12:$J$20</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$K$11</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$K$12:$K$20</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$F$11:$F$19</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$G$10</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$G$11:$G$19</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$H$10</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$H$11:$H$19</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$I$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$G$2</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$I$11:$I$19</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$J$10</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$J$11:$J$19</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$K$10</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$K$11:$K$19</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$K$11:$K$19</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$G$11</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$G$12:$G$20</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$H$11</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$H$12:$H$20</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$3</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$I$11</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$I$12:$I$20</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$J$11</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$J$12:$J$20</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$K$11</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$K$12:$K$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$G$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$G$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$G$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$H$2:$P$2</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$H$3:$P$3</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -98,7 +50,7 @@
     <t>Avg pH</t>
   </si>
   <si>
-    <t>Supplemental Table Y. Average pH associated with overlying water of each wetland region. Avg pH = average pH, STDev = standard deviation, n = number of replicate readings taken per region.</t>
+    <t>Supplemental Table 1. Average pH associated with overlying water of each wetland region. Avg pH = average pH, STDev = standard deviation, n = number of replicate readings taken per region.</t>
   </si>
 </sst>
 </file>

</xml_diff>